<commit_message>
integrate structure into veg matching and in clustering
</commit_message>
<xml_diff>
--- a/output/euicmuckplotassociations.xlsx
+++ b/output/euicmuckplotassociations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace2\USNVC\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979A1057-4928-4374-A4F2-92AB6AB69D03}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629E6D77-D5A0-488F-B3B2-5E56B67CB5E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allplotassociations" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="149">
   <si>
     <t>soilplot</t>
   </si>
@@ -286,21 +286,6 @@
     <t>Houghton.s20200701.01</t>
   </si>
   <si>
-    <t>marsh</t>
-  </si>
-  <si>
-    <t>fen</t>
-  </si>
-  <si>
-    <t>tamarack swamp</t>
-  </si>
-  <si>
-    <t>other swamp</t>
-  </si>
-  <si>
-    <t>reed canary grass</t>
-  </si>
-  <si>
     <t>Observation_ID</t>
   </si>
   <si>
@@ -469,23 +454,41 @@
     <t>Dasiphora fruticosa ssp. floribunda / Cladium mariscoides - Juncus balticus - (Rhynchospora capillacea) Fen</t>
   </si>
   <si>
-    <t>hardwood swamp1</t>
-  </si>
-  <si>
-    <t>hardwood swamp2</t>
-  </si>
-  <si>
-    <t>wet meadow1</t>
-  </si>
-  <si>
-    <t>wet meadow2</t>
+    <t>Salix nigra / (Cephalanthus occidentalis) Swamp Forest</t>
+  </si>
+  <si>
+    <t>01drained swamp</t>
+  </si>
+  <si>
+    <t>02silver maple buttonbush swamp</t>
+  </si>
+  <si>
+    <t>03silver maple green ash</t>
+  </si>
+  <si>
+    <t>04tamarack</t>
+  </si>
+  <si>
+    <t>05red maple dogwood lake sedge swamp</t>
+  </si>
+  <si>
+    <t>06fen</t>
+  </si>
+  <si>
+    <t>07marsh</t>
+  </si>
+  <si>
+    <t>08wet meadow</t>
+  </si>
+  <si>
+    <t>09reed canary grass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +627,12 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3546,17 +3555,15 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:C52"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G52" sqref="A1:G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3564,10 +3571,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D1" t="s">
         <v>72</v>
@@ -3587,10 +3594,10 @@
         <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3610,10 +3617,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3630,13 +3637,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -3653,13 +3660,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -3676,13 +3683,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -3699,13 +3706,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -3714,21 +3721,21 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>686814</v>
+        <v>685467</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -3737,67 +3744,67 @@
         <v>4</v>
       </c>
       <c r="F8">
-        <v>686814</v>
+        <v>685467</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>685467</v>
+        <v>688421</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>685467</v>
+        <v>686814</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -3806,21 +3813,21 @@
         <v>3</v>
       </c>
       <c r="F11">
-        <v>688421</v>
+        <v>686814</v>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -3829,21 +3836,21 @@
         <v>3</v>
       </c>
       <c r="F12">
-        <v>683201</v>
+        <v>686814</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -3860,13 +3867,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -3883,13 +3890,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -3898,21 +3905,21 @@
         <v>3</v>
       </c>
       <c r="F15">
-        <v>686869</v>
+        <v>683201</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -3921,21 +3928,21 @@
         <v>3</v>
       </c>
       <c r="F16">
-        <v>686869</v>
+        <v>683201</v>
       </c>
       <c r="G16" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -3944,21 +3951,21 @@
         <v>3</v>
       </c>
       <c r="F17">
-        <v>686869</v>
+        <v>683201</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>142</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -3967,21 +3974,21 @@
         <v>7</v>
       </c>
       <c r="F18">
-        <v>685728</v>
+        <v>686814</v>
       </c>
       <c r="G18" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>142</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -3990,21 +3997,21 @@
         <v>7</v>
       </c>
       <c r="F19">
-        <v>685728</v>
+        <v>686814</v>
       </c>
       <c r="G19" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>142</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -4013,21 +4020,21 @@
         <v>7</v>
       </c>
       <c r="F20">
-        <v>687037</v>
+        <v>892928</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" t="s">
         <v>142</v>
-      </c>
-      <c r="C21" t="s">
-        <v>84</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -4036,596 +4043,596 @@
         <v>7</v>
       </c>
       <c r="F21">
-        <v>690040</v>
+        <v>685467</v>
       </c>
       <c r="G21" t="s">
-        <v>143</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22">
-        <v>686101</v>
+        <v>683869</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D23">
         <v>4</v>
       </c>
       <c r="E23">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F23">
-        <v>687693</v>
+        <v>688421</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D24">
         <v>4</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F24">
-        <v>687693</v>
+        <v>688675</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D25">
         <v>4</v>
       </c>
       <c r="E25">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F25">
-        <v>687693</v>
+        <v>689089</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C26" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D26">
         <v>4</v>
       </c>
       <c r="E26">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F26">
-        <v>793415</v>
+        <v>689089</v>
       </c>
       <c r="G26" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D27">
         <v>4</v>
       </c>
       <c r="E27">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F27">
-        <v>793415</v>
+        <v>689089</v>
       </c>
       <c r="G27" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F28">
-        <v>685380</v>
+        <v>686788</v>
       </c>
       <c r="G28" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="D29">
         <v>5</v>
       </c>
       <c r="E29">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F29">
-        <v>689103</v>
+        <v>688421</v>
       </c>
       <c r="G29" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="D30">
         <v>5</v>
       </c>
       <c r="E30">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F30">
-        <v>689818</v>
+        <v>686814</v>
       </c>
       <c r="G30" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="D31">
         <v>5</v>
       </c>
       <c r="E31">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F31">
-        <v>689818</v>
+        <v>683201</v>
       </c>
       <c r="G31" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="C32" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D32">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E32">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F32">
-        <v>687693</v>
+        <v>686101</v>
       </c>
       <c r="G32" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
         <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D33">
         <v>6</v>
       </c>
       <c r="E33">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F33">
-        <v>687693</v>
+        <v>685728</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>134</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D34">
         <v>6</v>
       </c>
       <c r="E34">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F34">
-        <v>687693</v>
+        <v>685728</v>
       </c>
       <c r="G34" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D35">
         <v>6</v>
       </c>
       <c r="E35">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F35">
-        <v>687693</v>
+        <v>687037</v>
       </c>
       <c r="G35" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="D36">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E36">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F36">
-        <v>688421</v>
+        <v>690040</v>
       </c>
       <c r="G36" t="s">
-        <v>7</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="D37">
         <v>7</v>
       </c>
       <c r="E37">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F37">
-        <v>688675</v>
+        <v>685380</v>
       </c>
       <c r="G37" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="D38">
         <v>7</v>
       </c>
       <c r="E38">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F38">
-        <v>689089</v>
+        <v>689103</v>
       </c>
       <c r="G38" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="D39">
         <v>7</v>
       </c>
       <c r="E39">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F39">
-        <v>689089</v>
+        <v>689818</v>
       </c>
       <c r="G39" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="D40">
         <v>7</v>
       </c>
       <c r="E40">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F40">
-        <v>689089</v>
+        <v>689818</v>
       </c>
       <c r="G40" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
       <c r="D41">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E41">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F41">
-        <v>686788</v>
+        <v>687693</v>
       </c>
       <c r="G41" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="D42">
         <v>8</v>
       </c>
       <c r="E42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F42">
-        <v>688421</v>
+        <v>687693</v>
       </c>
       <c r="G42" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="D43">
         <v>8</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F43">
-        <v>683201</v>
+        <v>687693</v>
       </c>
       <c r="G43" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="C44" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="D44">
         <v>8</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F44">
-        <v>686101</v>
+        <v>687693</v>
       </c>
       <c r="G44" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="D45">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45">
-        <v>686190</v>
+        <v>687693</v>
       </c>
       <c r="G45" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C46" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="D46">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46">
-        <v>892928</v>
+        <v>687693</v>
       </c>
       <c r="G46" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C47" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="D47">
         <v>9</v>
@@ -4634,21 +4641,21 @@
         <v>1</v>
       </c>
       <c r="F47">
-        <v>686814</v>
+        <v>687693</v>
       </c>
       <c r="G47" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="D48">
         <v>9</v>
@@ -4657,21 +4664,21 @@
         <v>1</v>
       </c>
       <c r="F48">
-        <v>686869</v>
+        <v>793415</v>
       </c>
       <c r="G48" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="C49" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="D49">
         <v>9</v>
@@ -4680,21 +4687,21 @@
         <v>1</v>
       </c>
       <c r="F49">
-        <v>689615</v>
+        <v>793415</v>
       </c>
       <c r="G49" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="D50">
         <v>9</v>
@@ -4711,13 +4718,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="D51">
         <v>9</v>
@@ -4734,13 +4741,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="C52" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="D52">
         <v>9</v>
@@ -4757,10 +4764,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H75" xr:uid="{06CCA540-54C9-4CC5-A0F0-3B56285E3C80}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H75">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G52">
       <sortCondition ref="D1:D75"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>